<commit_message>
'900-1145PM' -> '900-1145 PM'
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67D3AF7-3F91-415F-8349-3AE9AD6E4188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D80286-0F48-4DB4-906E-A973D3702007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="870" windowWidth="16635" windowHeight="12030" tabRatio="698" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="4725" yWindow="210" windowWidth="16635" windowHeight="12030" tabRatio="778" firstSheet="2" activeTab="6" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="1200-245 PM" sheetId="5" r:id="rId4"/>
     <sheet name="300-545 PM" sheetId="6" r:id="rId5"/>
     <sheet name="600-845 PM" sheetId="7" r:id="rId6"/>
-    <sheet name="900-1145PM" sheetId="8" r:id="rId7"/>
+    <sheet name="900-1145 PM" sheetId="8" r:id="rId7"/>
     <sheet name="1200-245 AM" sheetId="9" r:id="rId8"/>
     <sheet name="300-545 AM" sheetId="10" r:id="rId9"/>
     <sheet name="Columns" sheetId="2" r:id="rId10"/>
@@ -1748,8 +1748,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1758,13 +1770,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1779,12 +1785,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2322,7 +2322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D396DD5C-31B0-418A-83C6-51CCF2B5706A}">
   <dimension ref="B1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
@@ -2349,44 +2349,44 @@
         <v>305</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="Q2" s="17" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="21" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="18"/>
+      <c r="R2" s="22"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
       <c r="Q3" s="14" t="s">
         <v>447</v>
       </c>
@@ -2399,172 +2399,172 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
       <c r="Q4" s="15" t="s">
         <v>448</v>
       </c>
       <c r="R4" s="13"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20179</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>352</v>
       </c>
       <c r="C6" s="19"/>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>442</v>
       </c>
       <c r="C9" s="19"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
@@ -2573,19 +2573,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
@@ -2600,6 +2587,19 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">
@@ -7091,8 +7091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A25666-08B9-424F-84A2-61B4C5A903D3}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added values for bp_loc_id and count_id for testing
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D80286-0F48-4DB4-906E-A973D3702007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A81CA7-DA16-4911-BE41-337DB6DD4F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="210" windowWidth="16635" windowHeight="12030" tabRatio="778" firstSheet="2" activeTab="6" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="930" yWindow="210" windowWidth="20430" windowHeight="12030" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1748,21 +1748,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1770,7 +1755,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1785,6 +1779,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2322,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D396DD5C-31B0-418A-83C6-51CCF2B5706A}">
   <dimension ref="B1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,48 +2349,50 @@
         <v>305</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="Q2" s="21" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="Q2" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="22"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
       <c r="Q3" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="R3" s="12"/>
+      <c r="R3" s="12">
+        <v>98765</v>
+      </c>
     </row>
     <row r="4" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
@@ -2399,172 +2401,174 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
       <c r="Q4" s="15" t="s">
         <v>448</v>
       </c>
-      <c r="R4" s="13"/>
+      <c r="R4" s="13">
+        <v>12345</v>
+      </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20179</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="17" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
@@ -2573,6 +2577,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
@@ -2589,17 +2604,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">
@@ -7091,7 +7095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A25666-08B9-424F-84A2-61B4C5A903D3}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Populated date field, for testing
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A81CA7-DA16-4911-BE41-337DB6DD4F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE4777F-2DD1-4020-A3DF-9090B1B7939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="210" windowWidth="20430" windowHeight="12030" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -1748,6 +1748,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1755,16 +1770,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1779,12 +1785,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2323,7 +2323,7 @@
   <dimension ref="B1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,45 +2348,47 @@
       <c r="B2" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="7">
+        <v>45229</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="Q2" s="16" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="21" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="17"/>
+      <c r="R2" s="22"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
       <c r="Q3" s="14" t="s">
         <v>447</v>
       </c>
@@ -2401,17 +2403,17 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
       <c r="Q4" s="15" t="s">
         <v>448</v>
       </c>
@@ -2420,155 +2422,155 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20179</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="21" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
@@ -2577,17 +2579,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
@@ -2604,6 +2595,17 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">

</xml_diff>

<commit_message>
bp_loc_id has type STRING
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE4777F-2DD1-4020-A3DF-9090B1B7939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DF5692-D417-43B6-8D95-A52D3ED7233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="210" windowWidth="20430" windowHeight="12030" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="450">
   <si>
     <t>Municipality</t>
   </si>
@@ -1467,6 +1467,9 @@
   </si>
   <si>
     <t>Count ID</t>
+  </si>
+  <si>
+    <t>98765-2023-10-30-v1'</t>
   </si>
 </sst>
 </file>
@@ -1736,9 +1739,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1748,21 +1748,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1770,7 +1755,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1786,6 +1780,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2323,7 +2326,7 @@
   <dimension ref="B1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2342,7 @@
     <col min="10" max="15" width="8.7109375" style="5"/>
     <col min="16" max="16" width="1.28515625" style="5" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" style="5" customWidth="1"/>
     <col min="19" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
@@ -2351,49 +2354,49 @@
       <c r="C2" s="7">
         <v>45229</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="21" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="Q2" s="21" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="Q2" s="15" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="22"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="Q3" s="14" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="Q3" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="R3" s="12">
-        <v>98765</v>
+      <c r="R3" s="28" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2403,21 +2406,21 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="Q4" s="15" t="s">
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="Q4" s="14" t="s">
         <v>448</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="12">
         <v>12345</v>
       </c>
     </row>
@@ -2426,151 +2429,151 @@
         <v>66</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20179</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>323</v>
       </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>324</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>325</v>
       </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
@@ -2579,6 +2582,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
@@ -2595,17 +2609,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">

</xml_diff>

<commit_message>
Fix to syntax of bp_loc_id string
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DF5692-D417-43B6-8D95-A52D3ED7233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A230A8F7-6726-4098-B759-7790FBA0E524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -1469,7 +1469,7 @@
     <t>Count ID</t>
   </si>
   <si>
-    <t>98765-2023-10-30-v1'</t>
+    <t>98765-2023-10-30-v1</t>
   </si>
 </sst>
 </file>
@@ -1748,6 +1748,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1786,9 +1789,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2354,48 +2354,48 @@
       <c r="C2" s="7">
         <v>45229</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="Q2" s="15" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="Q2" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="16"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
       <c r="Q3" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="R3" s="15" t="s">
         <v>449</v>
       </c>
     </row>
@@ -2406,17 +2406,17 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
       <c r="Q4" s="14" t="s">
         <v>448</v>
       </c>
@@ -2425,155 +2425,155 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20179</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">

</xml_diff>

<commit_message>
bp_loc_id has type INTEGER; count_id has type STRING
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A230A8F7-6726-4098-B759-7790FBA0E524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DF87C3-99C0-4095-B22A-8DE67D273315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -1552,7 +1552,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1687,26 +1687,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1739,9 +1724,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1751,6 +1733,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1758,16 +1755,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1782,12 +1770,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2326,7 +2308,7 @@
   <dimension ref="B1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,49 +2336,49 @@
       <c r="C2" s="7">
         <v>45229</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="22" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="Q2" s="16" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="Q2" s="20" t="s">
         <v>446</v>
       </c>
-      <c r="R2" s="17"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="Q3" s="13" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="Q3" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="R3" s="15" t="s">
-        <v>449</v>
+      <c r="R3" s="5">
+        <v>12345</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2406,174 +2388,174 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="Q4" s="14" t="s">
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="Q4" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="R4" s="12">
-        <v>12345</v>
+      <c r="R4" s="14" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
         <v>20179</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
     </row>
     <row r="6" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>352</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>442</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
@@ -2582,17 +2564,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
@@ -2609,6 +2580,17 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">

</xml_diff>

<commit_message>
Added comments text for testing
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet3.xlsx
+++ b/xlsx/sample-spreadsheet3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DF87C3-99C0-4095-B22A-8DE67D273315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE842F3-064E-49E7-838B-E825AA2BE60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="778" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="451">
   <si>
     <t>Municipality</t>
   </si>
@@ -1470,6 +1470,9 @@
   </si>
   <si>
     <t>98765-2023-10-30-v1</t>
+  </si>
+  <si>
+    <t>This is some text with an apostrophe in it: It's like this.</t>
   </si>
 </sst>
 </file>
@@ -2308,7 +2311,7 @@
   <dimension ref="B1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,7 +2396,9 @@
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="24"/>
+      <c r="J4" s="24" t="s">
+        <v>450</v>
+      </c>
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
       <c r="M4" s="24"/>

</xml_diff>